<commit_message>
park pick up money event
</commit_message>
<xml_diff>
--- a/Assets/Resources/excelData/AfterEvent.xlsx
+++ b/Assets/Resources/excelData/AfterEvent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>EventCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,10 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CareQuiz</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Choice</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -207,6 +203,30 @@
   </si>
   <si>
     <t>Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility-CareQuiz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Park-work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Park</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV016</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,15 +590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -628,21 +648,21 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -650,10 +670,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -661,10 +681,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -672,10 +692,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -683,90 +703,112 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
+      <c r="C19" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -781,10 +823,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -799,13 +844,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -819,53 +864,53 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
park walk event pick up item
</commit_message>
<xml_diff>
--- a/Assets/Resources/excelData/AfterEvent.xlsx
+++ b/Assets/Resources/excelData/AfterEvent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>EventCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +227,18 @@
   </si>
   <si>
     <t>EV016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Park</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -590,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -791,23 +803,34 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new game data reset
</commit_message>
<xml_diff>
--- a/Assets/Resources/excelData/AfterEvent.xlsx
+++ b/Assets/Resources/excelData/AfterEvent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>EventCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>EV019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fade Out</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -262,7 +274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +292,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -310,11 +330,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -618,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -641,15 +664,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -657,7 +680,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -668,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -676,24 +699,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -701,7 +724,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -712,7 +735,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -720,10 +743,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -731,13 +754,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
@@ -745,10 +768,10 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -756,21 +779,21 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
@@ -778,65 +801,65 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
@@ -844,7 +867,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
@@ -852,23 +875,34 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
main event black box ui
</commit_message>
<xml_diff>
--- a/Assets/Resources/excelData/AfterEvent.xlsx
+++ b/Assets/Resources/excelData/AfterEvent.xlsx
@@ -278,7 +278,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Text</t>
+    <t>Main Fade Out Persist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
main event ui black box
</commit_message>
<xml_diff>
--- a/Assets/Resources/excelData/AfterEvent.xlsx
+++ b/Assets/Resources/excelData/AfterEvent.xlsx
@@ -278,7 +278,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Main Fade Out Persist</t>
+    <t>Main Fade Out</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>